<commit_message>
add 8 more test cases for espn FantasyPage
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/espnFantasy.xlsx
+++ b/com.espn/src/test/resources/espnFantasy.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.espn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF235DE-1270-8942-9B36-EF64EB1F654C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7249B444-AB53-BA48-ABE1-62FE17282ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="NavBarMenu" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
+    <sheet name="URL" sheetId="2" r:id="rId2"/>
     <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>A</t>
   </si>
@@ -83,6 +83,39 @@
   </si>
   <si>
     <t>ESPN Fantasy App</t>
+  </si>
+  <si>
+    <t>https://fantasy.espn.com/basketball/welcome?addata=fantasy_home_nav_fba2022</t>
+  </si>
+  <si>
+    <t>expURL</t>
+  </si>
+  <si>
+    <t>https://fantasy.espn.com/hockey/welcome?addata=fhl_2022_fantasy_home_nav</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/fantasy/baseball/</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/fantasy/football/</t>
+  </si>
+  <si>
+    <t>https://fantasy.espn.com/free-prize-games</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/fantasy/basketball/</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/fantasy/hockey/</t>
+  </si>
+  <si>
+    <t>https://fantasy.espn.com/streak/en/</t>
+  </si>
+  <si>
+    <t>http://www.espn.com/espn/apps/fantasy</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/fantasy/</t>
   </si>
 </sst>
 </file>
@@ -443,13 +476,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -509,6 +542,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -584,14 +618,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add 6 more test cases for espn FantasyPage
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/espnFantasy.xlsx
+++ b/com.espn/src/test/resources/espnFantasy.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.espn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7249B444-AB53-BA48-ABE1-62FE17282ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB746E5-E1CA-D24C-8F3F-529D1A1F2F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="NavBarMenu" sheetId="1" r:id="rId1"/>
     <sheet name="URL" sheetId="2" r:id="rId2"/>
-    <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
+    <sheet name="CreateAccount" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
     <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>A</t>
   </si>
@@ -116,13 +116,40 @@
   </si>
   <si>
     <t>https://www.espn.com/fantasy/</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>mike34@yahoo.com</t>
+  </si>
+  <si>
+    <t>asdf8970</t>
+  </si>
+  <si>
+    <t>Jonathon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +162,14 @@
       <color rgb="FF202124"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,14 +189,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -620,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -691,14 +730,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{CECF1E96-EB00-1D46-BD0C-FA2D6A67C521}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{C9C286AE-3233-EB4B-BCC3-E6B7E3359C40}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{34F9E3A4-6057-1242-809C-87E4D4415EAC}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{DA64F942-2B04-8343-80F0-1104AA57CA84}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add 3 more test cases for espn FantasyPage
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/espnFantasy.xlsx
+++ b/com.espn/src/test/resources/espnFantasy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.espn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB746E5-E1CA-D24C-8F3F-529D1A1F2F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F821A9F3-F882-AC41-ACE5-EC61C930E04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>A</t>
   </si>
@@ -143,6 +143,30 @@
   </si>
   <si>
     <t>Jonathon</t>
+  </si>
+  <si>
+    <t>carla</t>
+  </si>
+  <si>
+    <t>brook</t>
+  </si>
+  <si>
+    <t>brook567@ymail.com</t>
+  </si>
+  <si>
+    <t>9876fdsa</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>1334348jdfhd</t>
+  </si>
+  <si>
+    <t>jas@</t>
   </si>
 </sst>
 </file>
@@ -730,10 +754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -828,12 +852,41 @@
         <v>30</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CECF1E96-EB00-1D46-BD0C-FA2D6A67C521}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{C9C286AE-3233-EB4B-BCC3-E6B7E3359C40}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{34F9E3A4-6057-1242-809C-87E4D4415EAC}"/>
     <hyperlink ref="C6" r:id="rId4" xr:uid="{DA64F942-2B04-8343-80F0-1104AA57CA84}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{2648F376-9E99-0241-9814-D0206A9D3D38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>